<commit_message>
Purchase Cost and Transaction report page format
</commit_message>
<xml_diff>
--- a/templates/Inventory.xlsx
+++ b/templates/Inventory.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Transactopm Report" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Transactopm Report'!$A$10:$N$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Transactopm Report'!$A$10:$O$10</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Transactopm Report'!$G$20</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Item Code</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>Purchase Cost</t>
   </si>
 </sst>
 </file>
@@ -226,17 +229,17 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -521,7 +524,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -536,14 +539,15 @@
     <col min="7" max="7" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -553,13 +557,14 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="5"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
-      <c r="N1" s="5"/>
-    </row>
-    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N1" s="4"/>
+      <c r="O1" s="5"/>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>15</v>
       </c>
@@ -571,13 +576,14 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="5"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
-      <c r="N2" s="5"/>
-    </row>
-    <row r="3" spans="1:14" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N2" s="4"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="1:15" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
@@ -585,51 +591,51 @@
       <c r="C3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="5"/>
-      <c r="N3" s="5"/>
-    </row>
-    <row r="4" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
+      <c r="K3" s="5"/>
+      <c r="O3" s="5"/>
+    </row>
+    <row r="4" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="6"/>
-      <c r="J4" s="5"/>
-      <c r="N4" s="5"/>
-    </row>
-    <row r="5" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
+      <c r="K4" s="5"/>
+      <c r="O4" s="5"/>
+    </row>
+    <row r="5" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="6"/>
-      <c r="J5" s="5"/>
-      <c r="N5" s="5"/>
-    </row>
-    <row r="6" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
+      <c r="K5" s="5"/>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="6"/>
-      <c r="J6" s="5"/>
-      <c r="N6" s="5"/>
-    </row>
-    <row r="7" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12"/>
+      <c r="K6" s="5"/>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="6"/>
-      <c r="J7" s="5"/>
-      <c r="N7" s="5"/>
-    </row>
-    <row r="8" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="K7" s="5"/>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="10"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="6"/>
-      <c r="J8" s="5"/>
-      <c r="N8" s="5"/>
-    </row>
-    <row r="9" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J9" s="5"/>
-      <c r="N9" s="5"/>
-    </row>
-    <row r="10" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="5"/>
+      <c r="O8" s="5"/>
+    </row>
+    <row r="9" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="5"/>
+      <c r="O9" s="5"/>
+    </row>
+    <row r="10" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -658,31 +664,34 @@
         <v>8</v>
       </c>
       <c r="J10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="L10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="O10" s="3" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A10:N10"/>
+  <autoFilter ref="A10:O10"/>
   <mergeCells count="7">
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>